<commit_message>
Added FACT components and remapped Dreamhouse App tests
</commit_message>
<xml_diff>
--- a/ProvarProject/templates/TestData.xlsx
+++ b/ProvarProject/templates/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16156\git\provardx\ProvarProject\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrdai\git\provardx\ProvarProject\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD9F04A-8A37-4C66-B5BF-C899B5F01B33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF21B323-D1E4-4A68-AEC6-1AB8C966077F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="4050" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="28800" windowHeight="15900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Property" sheetId="1" r:id="rId1"/>
@@ -445,26 +445,26 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.9296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.06640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.46484375" customWidth="1"/>
-    <col min="10" max="10" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.9296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.9296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.53125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.6640625" customWidth="1"/>
-    <col min="16" max="16" width="14.19921875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" customWidth="1"/>
+    <col min="10" max="10" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.6328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.6328125" customWidth="1"/>
+    <col min="16" max="16" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -517,7 +517,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -531,7 +531,7 @@
         <v>20</v>
       </c>
       <c r="E2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F2">
         <v>2</v>
@@ -569,17 +569,17 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="A1:D2"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.9296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -593,7 +593,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>22</v>
       </c>

</xml_diff>